<commit_message>
ce_data and pe_data are splitted, two strike prices for each
</commit_message>
<xml_diff>
--- a/option_chain_analysis.xlsx
+++ b/option_chain_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayank\Desktop\Python\NSEIndia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06255D51-E157-4010-82C0-E4971E0DEE77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4428DEC-0CAA-4C33-A0B1-37193A489177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>change</t>
   </si>
@@ -48,7 +48,10 @@
     <t>pchangeinOpenInterest</t>
   </si>
   <si>
-    <t>strikePrice</t>
+    <t>strikePrice_PE</t>
+  </si>
+  <si>
+    <t>strikePrice_CE</t>
   </si>
 </sst>
 </file>
@@ -84,9 +87,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,67 +378,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="7" max="7" width="19.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="19.44140625" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>